<commit_message>
SPARQL Wrapper 1st testing complete
</commit_message>
<xml_diff>
--- a/000000_Shakespeare.xlsx
+++ b/000000_Shakespeare.xlsx
@@ -4740,12 +4740,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>madsrdf:elementList{BNode}</t>
+          <t>identifiers:lccn{Literal}</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>N502e7a50ae9746c98916e9aabc06c12f</t>
+          <t>n 78095332</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -4782,12 +4782,12 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>identifiers:lccn{Literal}</t>
+          <t>identifiers:local{Literal}</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>n 78095332</t>
+          <t>(OCoLC)oca00230409</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -4824,12 +4824,12 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>identifiers:local{Literal}</t>
+          <t>madsrdf:adminMetadata{BNode}[0]</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>(OCoLC)oca00230409</t>
+          <t>Nacfef480aaf74e9484314c7ca6c191a0</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -4866,12 +4866,12 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>madsrdf:adminMetadata{BNode}[0]</t>
+          <t>madsrdf:adminMetadata{BNode}[1]</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Nc3321998b2e043f493fb7961b269789b</t>
+          <t>Ne25508050f1941deb39733c55e9cb99c</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -4908,12 +4908,12 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>madsrdf:adminMetadata{BNode}[1]</t>
+          <t>madsrdf:authoritativeLabel{Literal}</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Nc5bb36f5322a4b54a737112cc07e732e</t>
+          <t>Shakespeare, William, 1564-1616</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -4950,12 +4950,12 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>madsrdf:authoritativeLabel{Literal}</t>
+          <t>madsrdf:classification{BNode}</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Shakespeare, William, 1564-1616</t>
+          <t>N0444e13b49d249f3b83f0c2c3cb62fcc</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -4992,12 +4992,12 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>madsrdf:classification{BNode}</t>
+          <t>madsrdf:editorialNote{Literal}[0]</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Nb8fa42ab88f24637aa2920e9b98f5a21</t>
+          <t>[Machine-derived non-Latin script reference project.]</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -5034,12 +5034,12 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>madsrdf:editorialNote{Literal}[0]</t>
+          <t>madsrdf:editorialNote{Literal}[1]</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>[Machine-derived non-Latin script reference project.]</t>
+          <t>[Non-Latin script references not evaluated.]</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -5076,12 +5076,12 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>madsrdf:editorialNote{Literal}[1]</t>
+          <t>madsrdf:elementList{BNode}</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>[Non-Latin script references not evaluated.]</t>
+          <t>Nddeb2f938d184d05a72b279bd14e38c5</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>N088775e994ce4eaf9dfb9a6bd2d9197f</t>
+          <t>N0c8ebec910df49309938bb1bdf6f0a8e</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>N0c17664b9deb488a89f1c6fd1cd7b2ad</t>
+          <t>N1588af16bca348d4ae468510395866a1</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -5375,7 +5375,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>N0fb216fd1b974835a9dda7e0eb05ce5a</t>
+          <t>N19e15a35c2474f6f9f22de435b5303cc</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>N11db8fd6525c4137a274ebd3a156a18f</t>
+          <t>N1c5043d013204845b622b9f0638df021</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -5459,7 +5459,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>N12f39d6acd944c378ac3b233071cdcb3</t>
+          <t>N1e56584c61cf4b41aac4b5bb335c6b4f</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>N18482984ff954646a85c173fd1e5eca9</t>
+          <t>N1f2baddd41fa4286b9356e00ec1b2fc1</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>N26d07a805d3245a3bfa557c7cf3cf013</t>
+          <t>N218dd088b5af4fba8e3f362a015c9fc8</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -5585,7 +5585,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>N2cfbdfd758654db2afe26807f9704470</t>
+          <t>N29378936c2634d56abae188477b24ad0</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -5627,7 +5627,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>N2f9ab483d1f84f218fa1b024c6e1c9c1</t>
+          <t>N29390d8f376f4d7995f4d765a3f43d8c</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>N38fa2d8f6ae04361aa9ae4bebbb92d8a</t>
+          <t>N29ea8d73a0f343fa8a3494bd13d16126</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>N3fae8f9b57f9435f950c09e0f4db940e</t>
+          <t>N2d320fa4f00146b698ebe7e3085dc74f</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -5753,7 +5753,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>N4c520f663ef94a69996041cfa46f68c9</t>
+          <t>N384c5c0288324f348f0bce57a404ef9f</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -5795,7 +5795,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>N584a7b4810dd48a3b0b10d79a12985f6</t>
+          <t>N39c4f22990df4f0abb6c4f78fd96ba46</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -5837,7 +5837,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>N5cba66215a874eaba97b33c3fbff0f3c</t>
+          <t>N42a211cb33a942d086e37f64348154b9</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -5879,7 +5879,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>N655732f9e2c94eb0be8bd0be5f732dc0</t>
+          <t>N432a11bec3584e98b44e176509030dc2</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>N66200dc1674d45a9a64d9f9bc95133ab</t>
+          <t>N57ddb1be20d3473c83f23ea1052702cd</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -5963,7 +5963,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>N67aa0824297d479e82fe01d1965e60df</t>
+          <t>N5bf4d761d8084da8a86ebf04242ae6ce</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>N6c5539808c0943baac63b6e669050125</t>
+          <t>N6592243275ef4a31b1eafea5cea327bf</t>
         </is>
       </c>
       <c r="E128" t="n">
@@ -6047,7 +6047,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>N76fcccdefe8649948ae11bb090d476e1</t>
+          <t>N6a5cb71b2df14498b3e0edbe49e46abe</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>N817299e6c92b4cf3991a22d1895ccdef</t>
+          <t>N9cb4360fe75b4069910d74e3c681a0ab</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -6131,7 +6131,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>N8e461f8defe24c56969b927540c52fda</t>
+          <t>Nc1c893256de849e695d60c2259d0549d</t>
         </is>
       </c>
       <c r="E131" t="n">
@@ -6173,7 +6173,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Nacdd2937afcc4bb8be18418684142867</t>
+          <t>Nc618d4c972174c23ab304a22ebe29c17</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Nb77a9907acf446bd97b378eaa679c14c</t>
+          <t>Nc716d021012548c69267d560704e08cd</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -6257,7 +6257,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Nc81b07ad0fa04734aff002393069d29f</t>
+          <t>Ncddf89795f9243bb97fd2ed03b0bb290</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -6299,7 +6299,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Nccb12d6bbc9d43ecb03ec9b00b2e96c2</t>
+          <t>Ndbe3b12912924ec89e6a458670677b5a</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Nd883fa7955de4303bf55a353def89478</t>
+          <t>Ne6438f34a4dc49ae9f88b03a1f06acc5</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Ndcfefcda0de84bee9413203e895855be</t>
+          <t>Ned3088d95e774d629425d697bfd2d774</t>
         </is>
       </c>
       <c r="E137" t="n">
@@ -6425,7 +6425,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Ne7ccd3d028044c0dbb537aecceca35e8</t>
+          <t>Nf87fdca2968d4f5c8701feabc497ddaf</t>
         </is>
       </c>
       <c r="E138" t="n">
@@ -6467,7 +6467,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Nf672426bc8cc424099570b18d592ea92</t>
+          <t>Nf952a26ab9cc444bb3a5bf1adc3b032b</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -6509,7 +6509,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Nf78dac425235413fa496068f4bbb2c72</t>
+          <t>Nfa352adcaec643b0918a630320d46494</t>
         </is>
       </c>
       <c r="E140" t="n">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Nfe2df54db422418692e0d38df4b335ac</t>
+          <t>Nfa4f822cac414830818ddbd8068aa968</t>
         </is>
       </c>
       <c r="E141" t="n">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Nfefc3e74f0f14f7e9e483480700ebfdf</t>
+          <t>Nfe8ca67f0a3f40298d82e94381935080</t>
         </is>
       </c>
       <c r="E142" t="n">
@@ -6635,7 +6635,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>N05bc00cb44244cba97d79e13ea4f964f</t>
+          <t>N00cc50643eea4758a93ca5c56800dc15</t>
         </is>
       </c>
       <c r="E143" t="n">
@@ -6677,7 +6677,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>N062ad5fff6c74888abfe7ece035d1647</t>
+          <t>N022e413cd9ff4a19a0b4ddf283ab60e8</t>
         </is>
       </c>
       <c r="E144" t="n">
@@ -6719,7 +6719,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>N09a227e9a7d447c988a673bbd43500a2</t>
+          <t>N033aebe5a21e48dd98071561beefdc69</t>
         </is>
       </c>
       <c r="E145" t="n">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>N0ec6d071c2e0473a87cbba3dced7d992</t>
+          <t>N06c904d6c3dd4318b37316ceda6d22f9</t>
         </is>
       </c>
       <c r="E146" t="n">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>N100f0714badf470190a9fc424984fc78</t>
+          <t>N0c9514fac11c4229880e2692b7a7cf0b</t>
         </is>
       </c>
       <c r="E147" t="n">
@@ -6845,7 +6845,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>N12fb09774e214892ab2a9e1603a26610</t>
+          <t>N122c00a2c7bf47619287098d36bf2535</t>
         </is>
       </c>
       <c r="E148" t="n">
@@ -6887,7 +6887,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>N1836d8ef9a9c4329907ca7e00212bc31</t>
+          <t>N1375c828fc3145e1aa70d9aed3feac64</t>
         </is>
       </c>
       <c r="E149" t="n">
@@ -6929,7 +6929,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>N19a5f74f473c42b5a96b06d3ea5b94d3</t>
+          <t>N13b02b4c256b41fbbc68ba1c181f4336</t>
         </is>
       </c>
       <c r="E150" t="n">
@@ -6971,7 +6971,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>N1b113a57d0be4892a1fae0a431d196d2</t>
+          <t>N171319d3d6344114898147985a6ae699</t>
         </is>
       </c>
       <c r="E151" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>N225fd35994e249fdaed3a6dcac0dc48b</t>
+          <t>N1a08b9730bc1498fb0acbb4d8e6d8b51</t>
         </is>
       </c>
       <c r="E152" t="n">
@@ -7055,7 +7055,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>N22ee1a6c059a4945aae99d15be16d3da</t>
+          <t>N1a833ff4867b4d4d843841fcee965a57</t>
         </is>
       </c>
       <c r="E153" t="n">
@@ -7097,7 +7097,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>N231660fc8f994ffda07366e07e1b9826</t>
+          <t>N1ddb2d5a985a4a8393dc2f63c7ced84e</t>
         </is>
       </c>
       <c r="E154" t="n">
@@ -7139,7 +7139,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>N27fb5a1963e34a06990d0d98a66e8839</t>
+          <t>N278dd28bdaec4d4596a79ca28a9f2a76</t>
         </is>
       </c>
       <c r="E155" t="n">
@@ -7181,7 +7181,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>N2944c854d12d4aeda158a286041b76b4</t>
+          <t>N27b9bb6ae6b5449392341d4a1e598d20</t>
         </is>
       </c>
       <c r="E156" t="n">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>N2ae0a7b3f313453a8bbeda2e3eba3a2a</t>
+          <t>N29b1efe5a61043618ad3e817ae975ca2</t>
         </is>
       </c>
       <c r="E157" t="n">
@@ -7265,7 +7265,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>N2ed64049965f4a7187b2f50a1625bf3b</t>
+          <t>N2a59c02fc6c54863a05ad7f61a986fa1</t>
         </is>
       </c>
       <c r="E158" t="n">
@@ -7307,7 +7307,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>N30e83396ad8a49b3a8c234d74fbba140</t>
+          <t>N2a933bb190df49b98a2a7e631450fb6b</t>
         </is>
       </c>
       <c r="E159" t="n">
@@ -7349,7 +7349,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>N3d68712377c543f1a3af3546aab6270a</t>
+          <t>N2e156bdde52b4299af0b1a6765e3dba5</t>
         </is>
       </c>
       <c r="E160" t="n">
@@ -7391,7 +7391,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>N3f6c4267be0941f78780884a95b8fb97</t>
+          <t>N2f8efe4cbd194322bd9ecbe04d447b3e</t>
         </is>
       </c>
       <c r="E161" t="n">
@@ -7433,7 +7433,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>N40bb8a6de02948c0b4dd812c83234ced</t>
+          <t>N3116248cb3ad4e2785df4e1fb5820dd6</t>
         </is>
       </c>
       <c r="E162" t="n">
@@ -7475,7 +7475,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>N4144304e176344769dbf6731a883f43d</t>
+          <t>N342d962950e346c9912d06e574e8c144</t>
         </is>
       </c>
       <c r="E163" t="n">
@@ -7517,7 +7517,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>N44f36e3a02054350b3fc934d79d5862a</t>
+          <t>N3435d4a60d684cf49a4b3d33774919ad</t>
         </is>
       </c>
       <c r="E164" t="n">
@@ -7559,7 +7559,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>N4714cd1079074f6094420b9693d63da9</t>
+          <t>N34909322d15d4cf0a03c979f939054e3</t>
         </is>
       </c>
       <c r="E165" t="n">
@@ -7601,7 +7601,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>N4cb33c8c5c474f94a2b87a4e565ad0a4</t>
+          <t>N3b4c086e196a4347858aec1c14851b41</t>
         </is>
       </c>
       <c r="E166" t="n">
@@ -7643,7 +7643,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>N4f281cea16fe41bdbadb36f73045d14b</t>
+          <t>N3df1e1a864414a2aa6285b736d688dfd</t>
         </is>
       </c>
       <c r="E167" t="n">
@@ -7685,7 +7685,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>N4f2ec865b09a4d8d93aa233fabf303ee</t>
+          <t>N42de0cdb5d3a4740af8219f98374050e</t>
         </is>
       </c>
       <c r="E168" t="n">
@@ -7727,7 +7727,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>N52923bc86c1345fb81fc9d35b63f98c0</t>
+          <t>N4e37c3f02cd84feb95e47d111d23ac39</t>
         </is>
       </c>
       <c r="E169" t="n">
@@ -7769,7 +7769,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>N59e5b9c944d24635a4218d5833ffc826</t>
+          <t>N4e74922e08d84fe5a50d767f0b9de910</t>
         </is>
       </c>
       <c r="E170" t="n">
@@ -7811,7 +7811,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>N5c6dd3065aea43668a91bf2a32f16d52</t>
+          <t>N4f3116338d544011b9d5854704f46591</t>
         </is>
       </c>
       <c r="E171" t="n">
@@ -7853,7 +7853,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>N5dd6cbeb6a7b4ea1840f80abac9657fb</t>
+          <t>N5615fb2383d844778a194b6ba3d6abbb</t>
         </is>
       </c>
       <c r="E172" t="n">
@@ -7895,7 +7895,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>N5de9d598c88d4146b984c6436a68a89e</t>
+          <t>N5813f98bb9734cc2a95c366017afbe86</t>
         </is>
       </c>
       <c r="E173" t="n">
@@ -7937,7 +7937,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>N6447333c059445cf90d2c8dbe7842352</t>
+          <t>N59b475487f5d47cbb40d541de35aba7b</t>
         </is>
       </c>
       <c r="E174" t="n">
@@ -7979,7 +7979,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>N64b6ee7c14bf4e2dafdaf120ec5bae36</t>
+          <t>N5a2ae845908e45b695396e4d7a93305e</t>
         </is>
       </c>
       <c r="E175" t="n">
@@ -8021,7 +8021,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>N69949be264254160adc75d62f74051b3</t>
+          <t>N5a8919803d7e46739e0a81832f47375f</t>
         </is>
       </c>
       <c r="E176" t="n">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>N6df417f106c44c86ac422fdc748c9e02</t>
+          <t>N5c3fb6194d514d7a9b682b9350c60785</t>
         </is>
       </c>
       <c r="E177" t="n">
@@ -8105,7 +8105,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>N6fddbd410dbe4b53804168d7dd82f22a</t>
+          <t>N5c8c7d536bf64cebafdaea8759003edc</t>
         </is>
       </c>
       <c r="E178" t="n">
@@ -8147,7 +8147,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>N70d07401cd2d4c1c87b6f0bae5ba746f</t>
+          <t>N5d2fc96775c248e9b7bd7119bde56537</t>
         </is>
       </c>
       <c r="E179" t="n">
@@ -8189,7 +8189,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>N7339b41028c443aa91a0884ea40079ae</t>
+          <t>N5d8de3d425eb4ba995d5c67f05efb55f</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -8231,7 +8231,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>N7b673c3dbe9d4678ade2674d52267c23</t>
+          <t>N62113c3efd5348c6b46b6b4ff24e41d5</t>
         </is>
       </c>
       <c r="E181" t="n">
@@ -8273,7 +8273,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>N7ba9456ecde94c7b84f061d85b311dd1</t>
+          <t>N625b7e679cba4b779e6d130e2f75a99f</t>
         </is>
       </c>
       <c r="E182" t="n">
@@ -8315,7 +8315,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>N7d8e944bab0543bdae1cd5a1fda4401f</t>
+          <t>N66fbefaf636f4d0aaa45367eb7499c42</t>
         </is>
       </c>
       <c r="E183" t="n">
@@ -8357,7 +8357,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>N81acbcb64e5d495eaadd0a4f37c15090</t>
+          <t>N6d63d90b7a4b4447a294f5bf8c7ae742</t>
         </is>
       </c>
       <c r="E184" t="n">
@@ -8399,7 +8399,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>N83f51e7d703f4191a7d0e7d9f653c49c</t>
+          <t>N6df8c2316e4b4438b03eb1862e153e5d</t>
         </is>
       </c>
       <c r="E185" t="n">
@@ -8441,7 +8441,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>N8400bc873f734beebaa11d93b3ae8517</t>
+          <t>N74c4b727c8a14aaca28cb9bb9e2a0043</t>
         </is>
       </c>
       <c r="E186" t="n">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>N8655d10719334eec89b153f5ec9eb0e6</t>
+          <t>N74d0353f0e2243ddb0edfbda8694967c</t>
         </is>
       </c>
       <c r="E187" t="n">
@@ -8525,7 +8525,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>N9339c322259942b7804ea6e08dbf03dd</t>
+          <t>N7957515e2472466691579e68970415e3</t>
         </is>
       </c>
       <c r="E188" t="n">
@@ -8567,7 +8567,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>N93ec095820ca417fa6f86f2345b58748</t>
+          <t>N79dede66cf9443faa28d8f5fc36655fe</t>
         </is>
       </c>
       <c r="E189" t="n">
@@ -8609,7 +8609,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>N94c8c035e79449d78f4ce57a01fa842e</t>
+          <t>N7f06325161154aa2928a1d5cf205d764</t>
         </is>
       </c>
       <c r="E190" t="n">
@@ -8651,7 +8651,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>N9657b623a70b44f696cd191f7060c4dd</t>
+          <t>N8327d9da33a94c7cbd5101824b26f3fa</t>
         </is>
       </c>
       <c r="E191" t="n">
@@ -8693,7 +8693,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>N9668a882ab0944fd94aed9b1fb506395</t>
+          <t>N83f44bca96994eb8b81a54d550dd86cc</t>
         </is>
       </c>
       <c r="E192" t="n">
@@ -8735,7 +8735,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>N9a387192f49a40e4b645c9f5b4b69b36</t>
+          <t>N85ce9fcb07854d518743b3cc1d1e8e40</t>
         </is>
       </c>
       <c r="E193" t="n">
@@ -8777,7 +8777,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>N9b3415e9b81b49d5b3da124df26bca2d</t>
+          <t>N8618b511fa9847f2b1a3c258a82e8ddb</t>
         </is>
       </c>
       <c r="E194" t="n">
@@ -8819,7 +8819,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>N9b728f30685447af85d08ea3d0005f5d</t>
+          <t>N8937e65361354e4bab14e019c5e9d685</t>
         </is>
       </c>
       <c r="E195" t="n">
@@ -8861,7 +8861,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>N9cec72c513314648abd4e21d0ce83980</t>
+          <t>N969eb6914136456689f48c0f9b2556d7</t>
         </is>
       </c>
       <c r="E196" t="n">
@@ -8903,7 +8903,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>N9ddd22008bb64ee4a793c29da7a47400</t>
+          <t>N9a93f3e1c376404ea3b2f7e9593037c3</t>
         </is>
       </c>
       <c r="E197" t="n">
@@ -8945,7 +8945,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>N9de14494ac5344b28a2710bcae6fa619</t>
+          <t>Na53735b0219a4fe991831ee8b711cf43</t>
         </is>
       </c>
       <c r="E198" t="n">
@@ -8987,7 +8987,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>N9f20e9d586b64e2780c28dc80ce57af7</t>
+          <t>Na7082c4a119c4a8da6f222396872de85</t>
         </is>
       </c>
       <c r="E199" t="n">
@@ -9029,7 +9029,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Na088ede013214532a6f480a39af71254</t>
+          <t>Nabd4da8c2cde486b9bdf45d2f2439d4b</t>
         </is>
       </c>
       <c r="E200" t="n">
@@ -9071,7 +9071,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Na4e7a37f61944a09856c1f1cdb594d60</t>
+          <t>Nadb96b2ee80646b39b5e031dfcef6fed</t>
         </is>
       </c>
       <c r="E201" t="n">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Na56ffae780f04cf2bc066dedc5fa4bb6</t>
+          <t>Naea6011cc7324b68981a7ce87f93bf4b</t>
         </is>
       </c>
       <c r="E202" t="n">
@@ -9155,7 +9155,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Na8ce31be15d44a61a97646c396e52ca7</t>
+          <t>Naed0384160e74a2f9a07f61022e29e01</t>
         </is>
       </c>
       <c r="E203" t="n">
@@ -9197,7 +9197,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Nb270c2b505e54589a2c1707be5a1500c</t>
+          <t>Nb2e6e68c79ef4432a91dcf5616e0f79d</t>
         </is>
       </c>
       <c r="E204" t="n">
@@ -9239,7 +9239,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Nb39cd65d2ea64f608149187f5453eea0</t>
+          <t>Nb62057cf55774080a2dabd631fa46041</t>
         </is>
       </c>
       <c r="E205" t="n">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Nb6c21d175e814b398a84b31d0aa0cb84</t>
+          <t>Nb77aab3186a54f09896b3f73f74a7f6e</t>
         </is>
       </c>
       <c r="E206" t="n">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Nb717341180434c5a9ebc57cb42e794ac</t>
+          <t>Nbc97a3e93305496b9340a4505301f913</t>
         </is>
       </c>
       <c r="E207" t="n">
@@ -9365,7 +9365,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Nb7487ac941aa4ef08cd96be125fc2450</t>
+          <t>Nc27887bf48294cf1b1c908e8e8ca4a24</t>
         </is>
       </c>
       <c r="E208" t="n">
@@ -9407,7 +9407,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Nbcc43e4e45e8438bab46f2a4cf4f3048</t>
+          <t>Nc3842a6123f24e21b2c1afd0303bcb18</t>
         </is>
       </c>
       <c r="E209" t="n">
@@ -9449,7 +9449,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Nc07a2b2adf634ee6b5f0f8f784681b03</t>
+          <t>Nc54c60aa9d5249a8bc1d82cb2f76d11b</t>
         </is>
       </c>
       <c r="E210" t="n">
@@ -9491,7 +9491,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Nc7f7d5c34b6449a58c46323708c8b5bb</t>
+          <t>Nc56c14b1c65842809a1fa14ad2cc62f0</t>
         </is>
       </c>
       <c r="E211" t="n">
@@ -9533,7 +9533,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Nca9d71bd6dc441518050e36cce722a45</t>
+          <t>Nc93da544679549a6be2465ac6443da0c</t>
         </is>
       </c>
       <c r="E212" t="n">
@@ -9575,7 +9575,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Ncb1f4c655ffb4d56bc4f0a4f5bbedd76</t>
+          <t>Nce0a3be8e3be4fe58f717a5ceffe5311</t>
         </is>
       </c>
       <c r="E213" t="n">
@@ -9617,7 +9617,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Ncb7473c1b4fc4950b9b7fa7f670e546c</t>
+          <t>Ncfd54fd3df84498f84882977b7643299</t>
         </is>
       </c>
       <c r="E214" t="n">
@@ -9659,7 +9659,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Nd10ebe0d41984450b00f454dd50f82e1</t>
+          <t>Nd4ab71b2fc5e4c09a625641281b23f9c</t>
         </is>
       </c>
       <c r="E215" t="n">
@@ -9701,7 +9701,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Nd2c4304330024ee0bb211eaf6abcd41c</t>
+          <t>Ndf3dd0b7efef4c548c3b74b7017280fa</t>
         </is>
       </c>
       <c r="E216" t="n">
@@ -9743,7 +9743,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Nd700e73a5f1947d591784cd6350402e6</t>
+          <t>Ndff3bccf09eb4b1c80088d8b42c55fec</t>
         </is>
       </c>
       <c r="E217" t="n">
@@ -9785,7 +9785,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Nd828bdca5b5d4b47810d1680f82d1df8</t>
+          <t>Ne6ef84cecab649f79e82822b54fee082</t>
         </is>
       </c>
       <c r="E218" t="n">
@@ -9827,7 +9827,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Ne2d57a5b030241239614c697426e91f1</t>
+          <t>Ne7dc8fd162d648fbbdbfdf6ba77902ee</t>
         </is>
       </c>
       <c r="E219" t="n">
@@ -9869,7 +9869,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Ne4c19437e06749e5a9f34184490acfb3</t>
+          <t>Neb817e8ab5a247968aba74cfdeb95a44</t>
         </is>
       </c>
       <c r="E220" t="n">
@@ -9911,7 +9911,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Ne78d7c1a8d6b4f16a67afb2b0d375e85</t>
+          <t>Ned506370efe54119a083e242427e79da</t>
         </is>
       </c>
       <c r="E221" t="n">
@@ -9953,7 +9953,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Nf13249dda48345599af5ddf7586a31bc</t>
+          <t>Nede2cc8f496b4fcf88b279feaea2c8e7</t>
         </is>
       </c>
       <c r="E222" t="n">
@@ -9995,7 +9995,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Nf3e56f2d7c5f45c49faa37147d7b3b54</t>
+          <t>Nedf586cc26eb4a4284bdee5e6481e3cc</t>
         </is>
       </c>
       <c r="E223" t="n">
@@ -10037,7 +10037,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Nf41399ca17344a88b2393789a37e9203</t>
+          <t>Nf6223caf5ef048dd99a75f0406baa895</t>
         </is>
       </c>
       <c r="E224" t="n">
@@ -10079,7 +10079,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Nf4e03d00136b4335a988fe660d18ffb5</t>
+          <t>Nf8ac344732bc4895a5f2c3d21b1a05ed</t>
         </is>
       </c>
       <c r="E225" t="n">
@@ -10121,7 +10121,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Nf53b6558f9ab4bca899ae18842344c76</t>
+          <t>Nfc63b63077274e5abc4adc167ef7e7f3</t>
         </is>
       </c>
       <c r="E226" t="n">
@@ -10163,7 +10163,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Nfc74092fa51b49a98ab70fa427ca2971</t>
+          <t>Nfd6679a5286e496e99b32e80c2a01f19</t>
         </is>
       </c>
       <c r="E227" t="n">
@@ -10205,7 +10205,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Nfd2fa1e6111e41d690d34ef68c2fd423</t>
+          <t>Nffa49c200f99409f8826b019e970f58d</t>
         </is>
       </c>
       <c r="E228" t="n">
@@ -12389,7 +12389,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>N0148884dd5a541dfb7c67dfa2537e21f</t>
+          <t>N0d6ad63b5bb4453a95db29253a5d552b</t>
         </is>
       </c>
       <c r="E280" t="n">
@@ -12431,7 +12431,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Nf415347accce4ce9837f7b3004840a75</t>
+          <t>N3994486c8cb04f569d313f23cd048bfa</t>
         </is>
       </c>
       <c r="E281" t="n">
@@ -12809,7 +12809,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>N067d507323fa4f9d930583ebe8354cbd</t>
+          <t>N0042137156ae4c16bd06eba639bdf6c5</t>
         </is>
       </c>
       <c r="E290" t="n">
@@ -12851,7 +12851,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>N0977c15e96c5499ba5de8d2c884232d9</t>
+          <t>N06d264c45a344176a613740f9440e614</t>
         </is>
       </c>
       <c r="E291" t="n">
@@ -12893,7 +12893,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>N097a10f9759b4c8f8e3a26330548e5f0</t>
+          <t>N0f763539b9ba4721ace6fb94e6759ab9</t>
         </is>
       </c>
       <c r="E292" t="n">
@@ -12935,7 +12935,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>N0b09074036c54021b60f2c77586d4f58</t>
+          <t>N106150c942274cce9811949c40ac1053</t>
         </is>
       </c>
       <c r="E293" t="n">
@@ -12977,7 +12977,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>N0ff7eddb28ae4c0aab2c2a05d77a910d</t>
+          <t>N121823dd18754922b2919bf3582e839d</t>
         </is>
       </c>
       <c r="E294" t="n">
@@ -13019,7 +13019,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>N15933854bef8431186eef37db7bee3e5</t>
+          <t>N162b765f01254de7b8a3e5644d4e1db8</t>
         </is>
       </c>
       <c r="E295" t="n">
@@ -13061,7 +13061,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>N188851deb35542e5bfdfce535fe01235</t>
+          <t>N16d719d3afae4782bb5a81015aeed6c4</t>
         </is>
       </c>
       <c r="E296" t="n">
@@ -13103,7 +13103,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>N1f88629ef75744ef952e026f9793a501</t>
+          <t>N17723f4a6f3a4a06b53e6ff899d66adc</t>
         </is>
       </c>
       <c r="E297" t="n">
@@ -13145,7 +13145,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>N22c7d62a6c654187b78f32ededa20f1e</t>
+          <t>N17c493626bd549a48a65260e37d2af56</t>
         </is>
       </c>
       <c r="E298" t="n">
@@ -13187,7 +13187,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>N25aedee5a9314e5091c8ec0173418d1d</t>
+          <t>N1a289063e4d941dea13765bcbe3eb39b</t>
         </is>
       </c>
       <c r="E299" t="n">
@@ -13229,7 +13229,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>N28cea4712b9c43c0be6934b927b8d48c</t>
+          <t>N1c46f5ecd44d4204816f67a45fe32659</t>
         </is>
       </c>
       <c r="E300" t="n">
@@ -13271,7 +13271,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>N329b65b2a6a94b8882aba5c70923d196</t>
+          <t>N1d98bb2a3cb04423921c9cad559c2fc3</t>
         </is>
       </c>
       <c r="E301" t="n">
@@ -13313,7 +13313,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>N34158a1caf7148439bcc38b166895f81</t>
+          <t>N2133341d418b4db8b1dd8f53eaad43cf</t>
         </is>
       </c>
       <c r="E302" t="n">
@@ -13355,7 +13355,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>N3775dd1234b84ebdbcc57560f7222d77</t>
+          <t>N25d0c640874f423493e4b8876a0a910b</t>
         </is>
       </c>
       <c r="E303" t="n">
@@ -13397,7 +13397,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>N3a0d99cffba14846835b6406efaf2dec</t>
+          <t>N25d5773bbcec40188701cc6a120194e8</t>
         </is>
       </c>
       <c r="E304" t="n">
@@ -13439,7 +13439,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>N3dee3ec73fc149d6b999f4ebda61b4fa</t>
+          <t>N27afafc2b48b41b2846968f4af72bdf6</t>
         </is>
       </c>
       <c r="E305" t="n">
@@ -13481,7 +13481,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>N3ee4936c5a924a5ab984fd80f488dac7</t>
+          <t>N296c2afb210e4f6d937c9772ab2af319</t>
         </is>
       </c>
       <c r="E306" t="n">
@@ -13523,7 +13523,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>N420cd5956d72413d9b360f54252c198c</t>
+          <t>N2b8b3072e2254d0b9d841cdd45593d19</t>
         </is>
       </c>
       <c r="E307" t="n">
@@ -13565,7 +13565,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>N4608acedcefe4dafa88f48afeb17bf05</t>
+          <t>N2c2e165ff1964e72b15a386726ec91eb</t>
         </is>
       </c>
       <c r="E308" t="n">
@@ -13607,7 +13607,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>N46795306ad224bb98c0d0495293bd6d3</t>
+          <t>N360b8a64c3034a34b4f6b9039b8e0db8</t>
         </is>
       </c>
       <c r="E309" t="n">
@@ -13649,7 +13649,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>N4a66c1f25c2949c19a0259a349e2fa01</t>
+          <t>N3dbb40287b39487485ad2d3722f9a937</t>
         </is>
       </c>
       <c r="E310" t="n">
@@ -13691,7 +13691,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>N4b698f73b9124abbb9cac3f2d93a340d</t>
+          <t>N3f6a60a95405455d88f1be6b77368aa9</t>
         </is>
       </c>
       <c r="E311" t="n">
@@ -13733,7 +13733,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>N4b787c532a7a4767baf60f7a9f4a110d</t>
+          <t>N3f6efa1cb7e244f2a9d2cae4020dec52</t>
         </is>
       </c>
       <c r="E312" t="n">
@@ -13775,7 +13775,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>N50bd26ff3c9d4b92a75b87f17448354a</t>
+          <t>N3fa5b186e13548d78f7130586493fc87</t>
         </is>
       </c>
       <c r="E313" t="n">
@@ -13817,7 +13817,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>N50fd2aec34e94056894bafd574782cbb</t>
+          <t>N4015c208bfa64007b5543c4feef716b6</t>
         </is>
       </c>
       <c r="E314" t="n">
@@ -13859,7 +13859,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>N5559352eab49480bbe616de1880e1293</t>
+          <t>N4cb175db98f3463883cf9d8f7c53a5e5</t>
         </is>
       </c>
       <c r="E315" t="n">
@@ -13901,7 +13901,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>N56315d7c82dc4ddaa9d30bd7db975601</t>
+          <t>N4d5e67c901fc4fdab82dcba637f90ccc</t>
         </is>
       </c>
       <c r="E316" t="n">
@@ -13943,7 +13943,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>N566a8d0a65234b2c84c2fe2caa735761</t>
+          <t>N4ff73a846af54cd5a6500ac29a4a3282</t>
         </is>
       </c>
       <c r="E317" t="n">
@@ -13985,7 +13985,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>N58b60bd42d5e498e99c84bd804e88e1a</t>
+          <t>N54e902f72a92410a8b8495ca9f11c623</t>
         </is>
       </c>
       <c r="E318" t="n">
@@ -14027,7 +14027,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>N59e77a47e0a24a2d81f0da5941638da9</t>
+          <t>N60981493f542404f863dcc4a79be13f0</t>
         </is>
       </c>
       <c r="E319" t="n">
@@ -14069,7 +14069,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>N5f488ce29f774091a39c27dd4c1cf8d6</t>
+          <t>N61d041a249184ba1884417cb5297b7cb</t>
         </is>
       </c>
       <c r="E320" t="n">
@@ -14111,7 +14111,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>N5f7860c05bcb4adfb0abe1e7049a1fe4</t>
+          <t>N6290eeb5e1e247feb654412fc63246d9</t>
         </is>
       </c>
       <c r="E321" t="n">
@@ -14153,7 +14153,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>N61f73bb7fc8941e0aa8fc8f19b748198</t>
+          <t>N62b6871f584648c89c10c8516c9e2f22</t>
         </is>
       </c>
       <c r="E322" t="n">
@@ -14195,7 +14195,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>N6237b62ca7f14be5b41f6b394843e357</t>
+          <t>N6aeeb8e34d334b6d95cf174818ad7e07</t>
         </is>
       </c>
       <c r="E323" t="n">
@@ -14237,7 +14237,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>N6576d39412094d8486fc89fec705780b</t>
+          <t>N6b6370e50b594ca1997de2cc83597966</t>
         </is>
       </c>
       <c r="E324" t="n">
@@ -14279,7 +14279,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>N694d199a2fdc4b1da556fb389febf6bc</t>
+          <t>N6d48e9cdb8d1422f99abd3d0735609ca</t>
         </is>
       </c>
       <c r="E325" t="n">
@@ -14321,7 +14321,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>N69e4c48d917042d6aad776aba6296337</t>
+          <t>N6ee27dae56fb4cd5b1fc744eaf2ad975</t>
         </is>
       </c>
       <c r="E326" t="n">
@@ -14363,7 +14363,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>N6dd80989fbb6427d94c5eab450d4f80e</t>
+          <t>N7058e46fdc70494ca025543cb122cac1</t>
         </is>
       </c>
       <c r="E327" t="n">
@@ -14405,7 +14405,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>N7410818ec883499da36802d3ed6bc84e</t>
+          <t>N717ea09ca55e44679646d43c37f349cd</t>
         </is>
       </c>
       <c r="E328" t="n">
@@ -14447,7 +14447,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>N7556d77375b942a993920178bff7e869</t>
+          <t>N725b1074a60843c2acdfef3f355fc843</t>
         </is>
       </c>
       <c r="E329" t="n">
@@ -14489,7 +14489,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>N7b41c8a93543436db406323f858cce1e</t>
+          <t>N72bf822d32c745e5b6c0d58d1fdb39db</t>
         </is>
       </c>
       <c r="E330" t="n">
@@ -14531,7 +14531,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>N7f12c18badc3451888405ea16cf134c0</t>
+          <t>N73ccef812a714486b3822fd8c5ff5fac</t>
         </is>
       </c>
       <c r="E331" t="n">
@@ -14573,7 +14573,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>N7fd9f799a67b47e6beb98938ac252355</t>
+          <t>N743d2bad273e44b6853a3a2f49b607cc</t>
         </is>
       </c>
       <c r="E332" t="n">
@@ -14615,7 +14615,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>N8765859394e0460390e3aed6f04c4a16</t>
+          <t>N747a9e863701408aba8d1f14d76431a0</t>
         </is>
       </c>
       <c r="E333" t="n">
@@ -14657,7 +14657,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>N879b9ffc60b3400e8c8e3f56d983262b</t>
+          <t>N7fd141d85b7749b4adaa3ede9a177ffe</t>
         </is>
       </c>
       <c r="E334" t="n">
@@ -14699,7 +14699,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>N885e688d7f4f46fb8b43c32a8bef9c47</t>
+          <t>N851d80f3d9c94bd4af5b928810d74248</t>
         </is>
       </c>
       <c r="E335" t="n">
@@ -14741,7 +14741,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>N8c2f92eb2c44493ebabde8bba37c452f</t>
+          <t>N864ae8b278d44b9da6822cbc75f50af1</t>
         </is>
       </c>
       <c r="E336" t="n">
@@ -14783,7 +14783,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>N8dd09faed0894b72898127f04ae28d5d</t>
+          <t>N8679453fea904067834c6562209ee4ed</t>
         </is>
       </c>
       <c r="E337" t="n">
@@ -14825,7 +14825,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>N9c2b7f4ee9e74dc2990109d29eed599c</t>
+          <t>N89e8f1d79b9742cca91e3aba4b1c8b53</t>
         </is>
       </c>
       <c r="E338" t="n">
@@ -14867,7 +14867,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>N9cc2f76b64c34b5cb98513b201a44c8b</t>
+          <t>N8a6db8da4954484f938bf24af31caefb</t>
         </is>
       </c>
       <c r="E339" t="n">
@@ -14909,7 +14909,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>N9ccc62029e3c4f70b77c99c121c67353</t>
+          <t>N8af117fa9683497ca2a0cbeca9e3c23b</t>
         </is>
       </c>
       <c r="E340" t="n">
@@ -14951,7 +14951,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Na7b739e027ce4d92a1e12dd3c03f3ed5</t>
+          <t>N8d86008dbbc346e7adbece65ef6ee631</t>
         </is>
       </c>
       <c r="E341" t="n">
@@ -14993,7 +14993,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Na8f1d4b45f9248eaa1c31fa96141beb7</t>
+          <t>N909d4d2486da4b92a78c09720c235f08</t>
         </is>
       </c>
       <c r="E342" t="n">
@@ -15035,7 +15035,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Na942b5ac9dc34ce8b63eb6918d3b4099</t>
+          <t>N9106d6288a264e479c2397ebf3332714</t>
         </is>
       </c>
       <c r="E343" t="n">
@@ -15077,7 +15077,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Nabc2a50104554e2d9da943b10e1f6a30</t>
+          <t>N9126dcc3a73f48369f3ed3f3e801aa9a</t>
         </is>
       </c>
       <c r="E344" t="n">
@@ -15119,7 +15119,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Nacd823f3222448989bb4da230f0ab3f3</t>
+          <t>N91641a61a35f4424a6fb48dae045dbd6</t>
         </is>
       </c>
       <c r="E345" t="n">
@@ -15161,7 +15161,7 @@
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>Nb154549715f04051a40e98f6a4dd6908</t>
+          <t>Na058e0daf28f46cd83af74eb450c3117</t>
         </is>
       </c>
       <c r="E346" t="n">
@@ -15203,7 +15203,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>Nb3bd0599abaa4fb0a93ea9ce33459db5</t>
+          <t>Na4508b85799340329871f8d18c924e4b</t>
         </is>
       </c>
       <c r="E347" t="n">
@@ -15245,7 +15245,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Nb577cca79492492b9fc4f4a7c88d39f1</t>
+          <t>Nad2afa6da90a475fa042a5c4679e50ec</t>
         </is>
       </c>
       <c r="E348" t="n">
@@ -15287,7 +15287,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Nba24d99d98e94ffda9f14babaca09720</t>
+          <t>Nb9acf6f9c97a4d58b92732465a6fa7d3</t>
         </is>
       </c>
       <c r="E349" t="n">
@@ -15329,7 +15329,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>Nbebe20879c5445c7a3249dbcb555c504</t>
+          <t>Nba0fc2f9d9474a969fa11a55fc40c1c6</t>
         </is>
       </c>
       <c r="E350" t="n">
@@ -15371,7 +15371,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>Nc0b175c2b5c544608133cfb6cb3f22b8</t>
+          <t>Nba6b0441dc414b9f950576a32a888c7f</t>
         </is>
       </c>
       <c r="E351" t="n">
@@ -15413,7 +15413,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>Nc19d27572f6c47958ef85243a09cc08f</t>
+          <t>Nbbf9de464f7e4ce3bf38cd3551aaafb7</t>
         </is>
       </c>
       <c r="E352" t="n">
@@ -15455,7 +15455,7 @@
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>Nc56bca78659b4e84b0ddca73e680ee88</t>
+          <t>Nc179a5a215a243979cbbed157dc2ff49</t>
         </is>
       </c>
       <c r="E353" t="n">
@@ -15497,7 +15497,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Nc9c2b146f9404c559c06634f2bb45af4</t>
+          <t>Nc5a3e31f7a204e5ca2fc7df408325f54</t>
         </is>
       </c>
       <c r="E354" t="n">
@@ -15539,7 +15539,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Nca5395f4ac3f42a59147117b69730b83</t>
+          <t>Ncb9b8f743e0d4d1f8eec916fab34260e</t>
         </is>
       </c>
       <c r="E355" t="n">
@@ -15581,7 +15581,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>Ncee379528f374f7083430677a760cb63</t>
+          <t>Ncbff1b09380a41368d17233248520af3</t>
         </is>
       </c>
       <c r="E356" t="n">
@@ -15623,7 +15623,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Nd01f8b4d32214cd19d4845350640fceb</t>
+          <t>Ncc8caecf77e34ee6963e973190bf0fac</t>
         </is>
       </c>
       <c r="E357" t="n">
@@ -15665,7 +15665,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Nd1bac8d82c164bec861ef40fb624fb4b</t>
+          <t>Ncd7bfa0d4af242a58d01ee9f6526955c</t>
         </is>
       </c>
       <c r="E358" t="n">
@@ -15707,7 +15707,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>Nd28b2581a4864c7d890ea3a0a0756e87</t>
+          <t>Ncf85dca7623f4d7c8157eb43ee5f07db</t>
         </is>
       </c>
       <c r="E359" t="n">
@@ -15749,7 +15749,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>Nd79e59eafa874e7ab003305a13098123</t>
+          <t>Nd28e06cb4f704913b587cebc270e0d8f</t>
         </is>
       </c>
       <c r="E360" t="n">
@@ -15791,7 +15791,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Nd7e60386fec3466a96804bcf192ca756</t>
+          <t>Nd5c6836ceae748e996d82a295ea5a9ae</t>
         </is>
       </c>
       <c r="E361" t="n">
@@ -15833,7 +15833,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>Ndb3fe8da343a472e912f9e56cf18cb12</t>
+          <t>Nd955978da2c845c189e85bc86b75ae5a</t>
         </is>
       </c>
       <c r="E362" t="n">
@@ -15875,7 +15875,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Ndbb2b15d015f407fb6ae4bb6a09a2d46</t>
+          <t>Ne17ba019646940bbb65847fc82473bef</t>
         </is>
       </c>
       <c r="E363" t="n">
@@ -15917,7 +15917,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>Ndc20db5421fe49cfb9daa3deec32b675</t>
+          <t>Ne1eae16a5bf549f6a9031da4ff2d772a</t>
         </is>
       </c>
       <c r="E364" t="n">
@@ -15959,7 +15959,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Ne0df204e398b41aa82a055c85a54e869</t>
+          <t>Ne59d9bef978f4d54a43580551cde84fb</t>
         </is>
       </c>
       <c r="E365" t="n">
@@ -16001,7 +16001,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Ne1661833501e48f19bde753f8ebabc59</t>
+          <t>Nebe72466fb9b4eb28c47a43007130720</t>
         </is>
       </c>
       <c r="E366" t="n">
@@ -16043,7 +16043,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Ne63bce10867b4f199934ce2576739a41</t>
+          <t>Need52465f9c347008072cf4135d7b504</t>
         </is>
       </c>
       <c r="E367" t="n">
@@ -16085,7 +16085,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Ne666f6017c134127adcbd1e5e2fac8c6</t>
+          <t>Nef0fcc2fb5ac40149c85ed2ebf6c6299</t>
         </is>
       </c>
       <c r="E368" t="n">
@@ -16127,7 +16127,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>Ne6e0fdf244654b69a31e524387c83894</t>
+          <t>Nefa7fbe46a9d4c5cab57cb80742004a6</t>
         </is>
       </c>
       <c r="E369" t="n">
@@ -16169,7 +16169,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Nedf5c813617e409daa43288820d66ebd</t>
+          <t>Nefcef9dcc3ae41f6bd8447845b1ae778</t>
         </is>
       </c>
       <c r="E370" t="n">
@@ -16211,7 +16211,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>Nf327b91700874ddabe897fd8eb253415</t>
+          <t>Nf2b53f4dfe394085b22befe14c5fc394</t>
         </is>
       </c>
       <c r="E371" t="n">
@@ -16253,7 +16253,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>Nf54a0bd103df457b9d1f094bb91b5eac</t>
+          <t>Nf328405e43df4509a873b1e031839909</t>
         </is>
       </c>
       <c r="E372" t="n">
@@ -16295,7 +16295,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>Nfa64d2f9d2954b048d6b3d3d52c068d0</t>
+          <t>Nfc45a6c5b6c1489ba80c2f51df3586f4</t>
         </is>
       </c>
       <c r="E373" t="n">
@@ -16337,7 +16337,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>Nfbff42ac1817433795c55a7014728d96</t>
+          <t>Nfcc1ac71492642c99b8177e944ecc2bd</t>
         </is>
       </c>
       <c r="E374" t="n">
@@ -16379,7 +16379,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>Nfd3ae67e000d425a8ec0f71ac8255e7f</t>
+          <t>Nfd976f39fc03449d9a16c93116d49278</t>
         </is>
       </c>
       <c r="E375" t="n">

</xml_diff>